<commit_message>
save new functional for mega delivery distance
</commit_message>
<xml_diff>
--- a/platform_scrapper/data/cannabis_used_IDs.xlsx
+++ b/platform_scrapper/data/cannabis_used_IDs.xlsx
@@ -6929,8 +6929,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N716"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:XFD133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9994,7 +9994,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>135</v>
       </c>
@@ -10110,7 +10110,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>91</v>
       </c>
@@ -10264,7 +10264,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>250</v>
       </c>
@@ -10293,7 +10293,7 @@
         <v>2111</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>75</v>
       </c>
@@ -10354,7 +10354,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>28</v>
       </c>
@@ -10383,7 +10383,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>135</v>
       </c>
@@ -10412,7 +10412,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>394</v>
       </c>
@@ -10441,7 +10441,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>28</v>
       </c>
@@ -10624,7 +10624,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>73</v>
       </c>
@@ -10711,7 +10711,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>28</v>
       </c>
@@ -10772,7 +10772,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>18</v>
       </c>
@@ -10862,7 +10862,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>33</v>
       </c>
@@ -10891,7 +10891,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>486</v>
       </c>
@@ -10972,7 +10972,7 @@
         <v>15195013797</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>127</v>
       </c>
@@ -11001,7 +11001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>69</v>
       </c>
@@ -11030,7 +11030,7 @@
         <v>2126</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>552</v>
       </c>
@@ -11059,7 +11059,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>250</v>
       </c>
@@ -11088,7 +11088,7 @@
         <v>2112</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>296</v>
       </c>
@@ -11117,7 +11117,7 @@
         <v>2112</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>38</v>
       </c>
@@ -11140,7 +11140,7 @@
         <v>14162664420</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>51</v>
       </c>
@@ -11166,7 +11166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>50</v>
       </c>
@@ -11192,7 +11192,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>585</v>
       </c>
@@ -11215,7 +11215,7 @@
         <v>17053861264</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>35</v>
       </c>
@@ -11273,7 +11273,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>461</v>
       </c>
@@ -11325,7 +11325,7 @@
         <v>14164311333</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>33</v>
       </c>
@@ -11348,7 +11348,7 @@
         <v>14165193555</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>28</v>
       </c>
@@ -11371,7 +11371,7 @@
         <v>14167672225</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>33</v>
       </c>
@@ -11397,7 +11397,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>33</v>
       </c>
@@ -11423,7 +11423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>35</v>
       </c>
@@ -11449,7 +11449,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>28</v>
       </c>
@@ -11472,7 +11472,7 @@
         <v>14168678888</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>356</v>
       </c>
@@ -11498,7 +11498,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>621</v>
       </c>
@@ -11524,7 +11524,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>625</v>
       </c>
@@ -11910,7 +11910,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>127</v>
       </c>
@@ -11936,7 +11936,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>28</v>
       </c>
@@ -11962,7 +11962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>134</v>
       </c>
@@ -11982,7 +11982,7 @@
         <v>15199422828</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>659</v>
       </c>
@@ -12005,7 +12005,7 @@
         <v>19059854898</v>
       </c>
     </row>
-    <row r="176" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>663</v>
       </c>
@@ -12028,7 +12028,7 @@
         <v>12267836286</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>673</v>
       </c>
@@ -12054,7 +12054,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>485</v>
       </c>
@@ -12077,7 +12077,7 @@
         <v>19055711842</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>65</v>
       </c>
@@ -12132,7 +12132,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>51</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>16138294111</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>686</v>
       </c>
@@ -12181,7 +12181,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>53</v>
       </c>
@@ -12207,7 +12207,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>57</v>
       </c>
@@ -12230,7 +12230,7 @@
         <v>15139227020</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>28</v>
       </c>
@@ -12256,7 +12256,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>161</v>
       </c>
@@ -12282,7 +12282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>28</v>
       </c>
@@ -12308,7 +12308,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>28</v>
       </c>
@@ -12334,7 +12334,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>60</v>
       </c>
@@ -12357,7 +12357,7 @@
         <v>19057996001</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>82</v>
       </c>
@@ -12383,7 +12383,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>87</v>
       </c>
@@ -12406,7 +12406,7 @@
         <v>18072150047</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>63</v>
       </c>
@@ -12487,7 +12487,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="195" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>38</v>
       </c>
@@ -12510,7 +12510,7 @@
         <v>14167524242</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>28</v>
       </c>
@@ -12536,7 +12536,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="197" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>79</v>
       </c>
@@ -12562,7 +12562,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="198" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>732</v>
       </c>
@@ -12588,7 +12588,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="199" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>47</v>
       </c>
@@ -12614,7 +12614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="200" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>91</v>
       </c>
@@ -12640,7 +12640,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="201" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>51</v>
       </c>
@@ -12666,7 +12666,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="202" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>745</v>
       </c>
@@ -12689,7 +12689,7 @@
         <v>16135263420</v>
       </c>
     </row>
-    <row r="203" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>99</v>
       </c>
@@ -12712,7 +12712,7 @@
         <v>15196019873</v>
       </c>
     </row>
-    <row r="204" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>35</v>
       </c>
@@ -12735,7 +12735,7 @@
         <v>19052087508</v>
       </c>
     </row>
-    <row r="205" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>28</v>
       </c>
@@ -12761,7 +12761,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="206" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>757</v>
       </c>
@@ -12787,7 +12787,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>82</v>
       </c>
@@ -12813,7 +12813,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="208" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>765</v>
       </c>
@@ -12836,7 +12836,7 @@
         <v>18077279830</v>
       </c>
     </row>
-    <row r="209" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>28</v>
       </c>
@@ -12978,7 +12978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="214" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>75</v>
       </c>
@@ -13004,7 +13004,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="215" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>394</v>
       </c>
@@ -13030,7 +13030,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="216" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>79</v>
       </c>
@@ -13053,7 +13053,7 @@
         <v>16133928655</v>
       </c>
     </row>
-    <row r="217" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>47</v>
       </c>
@@ -13076,7 +13076,7 @@
         <v>16135999209</v>
       </c>
     </row>
-    <row r="218" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>783</v>
       </c>
@@ -13125,7 +13125,7 @@
         <v>14165460810</v>
       </c>
     </row>
-    <row r="220" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>75</v>
       </c>
@@ -13148,7 +13148,7 @@
         <v>19052400192</v>
       </c>
     </row>
-    <row r="221" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>35</v>
       </c>
@@ -13174,7 +13174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="222" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>35</v>
       </c>
@@ -13200,7 +13200,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="223" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>65</v>
       </c>
@@ -13226,7 +13226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="224" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>65</v>
       </c>
@@ -13284,7 +13284,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="226" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>65</v>
       </c>
@@ -13339,7 +13339,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="228" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>35</v>
       </c>
@@ -13365,7 +13365,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="229" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>563</v>
       </c>
@@ -13388,7 +13388,7 @@
         <v>17053224210</v>
       </c>
     </row>
-    <row r="230" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>820</v>
       </c>
@@ -13414,7 +13414,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="231" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>225</v>
       </c>
@@ -13440,7 +13440,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="232" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>826</v>
       </c>
@@ -13518,7 +13518,7 @@
         <v>14374101420</v>
       </c>
     </row>
-    <row r="235" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>28</v>
       </c>
@@ -13573,7 +13573,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="237" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>484</v>
       </c>
@@ -13799,7 +13799,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="245" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>60</v>
       </c>
@@ -13822,7 +13822,7 @@
         <v>19054532899</v>
       </c>
     </row>
-    <row r="246" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>56</v>
       </c>
@@ -13871,7 +13871,7 @@
         <v>19055476002</v>
       </c>
     </row>
-    <row r="248" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>846</v>
       </c>
@@ -13894,7 +13894,7 @@
         <v>18078538888</v>
       </c>
     </row>
-    <row r="249" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>28</v>
       </c>
@@ -13914,7 +13914,7 @@
         <v>14165335773</v>
       </c>
     </row>
-    <row r="250" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>35</v>
       </c>
@@ -13937,7 +13937,7 @@
         <v>19055458559</v>
       </c>
     </row>
-    <row r="251" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>51</v>
       </c>
@@ -13958,7 +13958,7 @@
       </c>
       <c r="I251"/>
     </row>
-    <row r="252" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>885</v>
       </c>
@@ -13981,7 +13981,7 @@
         <v>16134322288</v>
       </c>
     </row>
-    <row r="253" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>621</v>
       </c>
@@ -14007,7 +14007,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="254" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>99</v>
       </c>
@@ -14033,7 +14033,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="255" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>73</v>
       </c>
@@ -14059,7 +14059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="256" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>57</v>
       </c>
@@ -14082,7 +14082,7 @@
         <v>17055039818</v>
       </c>
     </row>
-    <row r="257" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>28</v>
       </c>
@@ -14108,7 +14108,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="258" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>26</v>
       </c>
@@ -14134,7 +14134,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="259" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>178</v>
       </c>
@@ -14160,7 +14160,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="260" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>912</v>
       </c>
@@ -14186,7 +14186,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="261" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>915</v>
       </c>
@@ -14212,7 +14212,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="262" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>60</v>
       </c>
@@ -14235,7 +14235,7 @@
         <v>19057963781</v>
       </c>
     </row>
-    <row r="263" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>60</v>
       </c>
@@ -14258,7 +14258,7 @@
         <v>12899486326</v>
       </c>
     </row>
-    <row r="264" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>13</v>
       </c>
@@ -14281,7 +14281,7 @@
         <v>12893374422</v>
       </c>
     </row>
-    <row r="265" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>13</v>
       </c>
@@ -14304,7 +14304,7 @@
         <v>12893371212</v>
       </c>
     </row>
-    <row r="266" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>126</v>
       </c>
@@ -14330,7 +14330,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="267" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>127</v>
       </c>
@@ -14353,7 +14353,7 @@
         <v>14165465626</v>
       </c>
     </row>
-    <row r="268" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>355</v>
       </c>
@@ -14379,7 +14379,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="269" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>184</v>
       </c>
@@ -14402,7 +14402,7 @@
         <v>15198247358</v>
       </c>
     </row>
-    <row r="270" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>184</v>
       </c>
@@ -14428,7 +14428,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="271" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>35</v>
       </c>
@@ -14451,7 +14451,7 @@
         <v>19055451317</v>
       </c>
     </row>
-    <row r="272" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>35</v>
       </c>
@@ -14477,7 +14477,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="273" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>96</v>
       </c>
@@ -14503,7 +14503,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="274" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>216</v>
       </c>
@@ -14529,7 +14529,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="275" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>47</v>
       </c>
@@ -14552,7 +14552,7 @@
         <v>16135910985</v>
       </c>
     </row>
-    <row r="276" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>55</v>
       </c>
@@ -14578,7 +14578,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="277" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>55</v>
       </c>
@@ -14601,7 +14601,7 @@
         <v>15482884318</v>
       </c>
     </row>
-    <row r="278" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>55</v>
       </c>
@@ -14624,7 +14624,7 @@
         <v>15198960644</v>
       </c>
     </row>
-    <row r="279" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>99</v>
       </c>
@@ -14647,7 +14647,7 @@
         <v>15193049999</v>
       </c>
     </row>
-    <row r="280" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>99</v>
       </c>
@@ -14673,7 +14673,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="281" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>56</v>
       </c>
@@ -14696,7 +14696,7 @@
         <v>19056931023</v>
       </c>
     </row>
-    <row r="282" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>135</v>
       </c>
@@ -14722,7 +14722,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="283" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>135</v>
       </c>
@@ -14748,7 +14748,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="284" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>967</v>
       </c>
@@ -14771,7 +14771,7 @@
         <v>16473989100</v>
       </c>
     </row>
-    <row r="285" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>82</v>
       </c>
@@ -14794,7 +14794,7 @@
         <v>16473989100</v>
       </c>
     </row>
-    <row r="286" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>82</v>
       </c>
@@ -14817,7 +14817,7 @@
         <v>16473685992</v>
       </c>
     </row>
-    <row r="287" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>75</v>
       </c>
@@ -14840,7 +14840,7 @@
         <v>19055768558</v>
       </c>
     </row>
-    <row r="288" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>51</v>
       </c>
@@ -14866,7 +14866,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="289" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>51</v>
       </c>
@@ -14889,7 +14889,7 @@
         <v>16135140575</v>
       </c>
     </row>
-    <row r="290" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>51</v>
       </c>
@@ -14915,7 +14915,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="291" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>45</v>
       </c>
@@ -14938,7 +14938,7 @@
         <v>16137445321</v>
       </c>
     </row>
-    <row r="292" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>38</v>
       </c>
@@ -14964,7 +14964,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="293" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>988</v>
       </c>
@@ -14987,7 +14987,7 @@
         <v>16136959165</v>
       </c>
     </row>
-    <row r="294" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>297</v>
       </c>
@@ -15013,7 +15013,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="295" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>341</v>
       </c>
@@ -15036,7 +15036,7 @@
         <v>15196377772</v>
       </c>
     </row>
-    <row r="296" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>268</v>
       </c>
@@ -15062,7 +15062,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="297" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>268</v>
       </c>
@@ -15088,7 +15088,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="298" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>73</v>
       </c>
@@ -15114,7 +15114,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="299" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>28</v>
       </c>
@@ -15140,7 +15140,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="300" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>28</v>
       </c>
@@ -15166,7 +15166,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="301" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>28</v>
       </c>
@@ -15189,7 +15189,7 @@
         <v>14165150009</v>
       </c>
     </row>
-    <row r="302" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>28</v>
       </c>
@@ -15215,7 +15215,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="303" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>28</v>
       </c>
@@ -15351,7 +15351,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="308" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>76</v>
       </c>
@@ -15403,7 +15403,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="310" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>76</v>
       </c>
@@ -15426,7 +15426,7 @@
         <v>15197831362</v>
       </c>
     </row>
-    <row r="311" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>121</v>
       </c>
@@ -15452,7 +15452,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="312" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>121</v>
       </c>
@@ -15475,7 +15475,7 @@
         <v>15199726146</v>
       </c>
     </row>
-    <row r="313" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>222</v>
       </c>
@@ -15501,7 +15501,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="314" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>511</v>
       </c>
@@ -15585,7 +15585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="317" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>28</v>
       </c>
@@ -15611,7 +15611,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="318" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>1043</v>
       </c>
@@ -15634,7 +15634,7 @@
         <v>12267224367</v>
       </c>
     </row>
-    <row r="319" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>90</v>
       </c>
@@ -15689,7 +15689,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="321" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>28</v>
       </c>
@@ -15712,7 +15712,7 @@
         <v>14165158868</v>
       </c>
     </row>
-    <row r="322" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>95</v>
       </c>
@@ -15799,7 +15799,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="325" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>60</v>
       </c>
@@ -15883,7 +15883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="328" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>28</v>
       </c>
@@ -15961,7 +15961,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="331" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>161</v>
       </c>
@@ -15987,7 +15987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="332" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>28</v>
       </c>
@@ -16013,7 +16013,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="333" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>28</v>
       </c>
@@ -16031,7 +16031,7 @@
       </c>
       <c r="I333"/>
     </row>
-    <row r="334" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>60</v>
       </c>
@@ -16057,7 +16057,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="335" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>60</v>
       </c>
@@ -16083,7 +16083,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="336" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>190</v>
       </c>
@@ -16109,7 +16109,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="337" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>33</v>
       </c>
@@ -16135,7 +16135,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="338" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>78</v>
       </c>
@@ -16161,7 +16161,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="339" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>184</v>
       </c>
@@ -16187,7 +16187,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="340" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>184</v>
       </c>
@@ -16213,7 +16213,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="341" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>65</v>
       </c>
@@ -16239,7 +16239,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="342" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>64</v>
       </c>
@@ -16265,7 +16265,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="343" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>82</v>
       </c>
@@ -16291,7 +16291,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="344" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>134</v>
       </c>
@@ -16317,7 +16317,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="345" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>75</v>
       </c>
@@ -16343,7 +16343,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="346" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>51</v>
       </c>
@@ -16369,7 +16369,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="347" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>38</v>
       </c>
@@ -16395,7 +16395,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="348" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>82</v>
       </c>
@@ -16421,7 +16421,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="349" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>28</v>
       </c>
@@ -16447,7 +16447,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="350" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>82</v>
       </c>
@@ -16473,7 +16473,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="351" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>28</v>
       </c>
@@ -16499,7 +16499,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="352" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>51</v>
       </c>
@@ -16525,7 +16525,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="353" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>1139</v>
       </c>
@@ -16551,7 +16551,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="354" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>28</v>
       </c>
@@ -16577,7 +16577,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="355" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>57</v>
       </c>
@@ -16603,7 +16603,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="356" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>1149</v>
       </c>
@@ -16629,7 +16629,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="357" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>185</v>
       </c>
@@ -16655,7 +16655,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="358" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>119</v>
       </c>
@@ -16681,7 +16681,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="359" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>461</v>
       </c>
@@ -16707,7 +16707,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="360" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>52</v>
       </c>
@@ -16733,7 +16733,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="361" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>75</v>
       </c>
@@ -16904,7 +16904,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="367" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>75</v>
       </c>
@@ -16930,7 +16930,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="368" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>28</v>
       </c>
@@ -16956,7 +16956,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="369" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>63</v>
       </c>
@@ -17008,7 +17008,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="371" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>47</v>
       </c>
@@ -17034,7 +17034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="372" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>28</v>
       </c>
@@ -17060,7 +17060,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="373" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>296</v>
       </c>
@@ -17109,7 +17109,7 @@
         <v>14167629922</v>
       </c>
     </row>
-    <row r="375" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>1197</v>
       </c>
@@ -17132,7 +17132,7 @@
         <v>17056653747</v>
       </c>
     </row>
-    <row r="376" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>121</v>
       </c>
@@ -17158,7 +17158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="377" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>26</v>
       </c>
@@ -17210,7 +17210,7 @@
         <v>13435881547</v>
       </c>
     </row>
-    <row r="379" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>28</v>
       </c>
@@ -17260,7 +17260,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="381" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>28</v>
       </c>
@@ -17283,7 +17283,7 @@
         <v>14378808271</v>
       </c>
     </row>
-    <row r="382" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>60</v>
       </c>
@@ -17303,7 +17303,7 @@
         <v>14167369014</v>
       </c>
     </row>
-    <row r="383" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>82</v>
       </c>
@@ -17323,7 +17323,7 @@
         <v>14167369014</v>
       </c>
     </row>
-    <row r="384" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>161</v>
       </c>
@@ -17349,7 +17349,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="385" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>28</v>
       </c>
@@ -17375,7 +17375,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="386" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>99</v>
       </c>
@@ -17401,7 +17401,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="387" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>99</v>
       </c>
@@ -17427,7 +17427,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="388" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>631</v>
       </c>
@@ -17453,7 +17453,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="389" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>1239</v>
       </c>
@@ -17479,7 +17479,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="390" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>1242</v>
       </c>
@@ -17505,7 +17505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="391" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>134</v>
       </c>
@@ -17531,7 +17531,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="392" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>51</v>
       </c>
@@ -17557,7 +17557,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="393" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>167</v>
       </c>
@@ -17583,7 +17583,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="394" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>45</v>
       </c>
@@ -17606,7 +17606,7 @@
         <v>16134214200</v>
       </c>
     </row>
-    <row r="395" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>65</v>
       </c>
@@ -17632,7 +17632,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="396" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>91</v>
       </c>
@@ -17655,7 +17655,7 @@
         <v>13438805588</v>
       </c>
     </row>
-    <row r="397" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>53</v>
       </c>
@@ -17759,7 +17759,7 @@
         <v>14167785659</v>
       </c>
     </row>
-    <row r="401" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>105</v>
       </c>
@@ -17785,7 +17785,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="402" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>1265</v>
       </c>
@@ -17811,7 +17811,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="403" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>75</v>
       </c>
@@ -17837,7 +17837,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="404" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>65</v>
       </c>
@@ -17863,7 +17863,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="405" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>76</v>
       </c>
@@ -17889,7 +17889,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="406" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>268</v>
       </c>
@@ -17944,7 +17944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="408" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>635</v>
       </c>
@@ -17967,7 +17967,7 @@
         <v>18074641851</v>
       </c>
     </row>
-    <row r="409" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>635</v>
       </c>
@@ -17990,7 +17990,7 @@
         <v>18074641851</v>
       </c>
     </row>
-    <row r="410" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>80</v>
       </c>
@@ -18016,7 +18016,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="411" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>99</v>
       </c>
@@ -18039,7 +18039,7 @@
         <v>15196529595</v>
       </c>
     </row>
-    <row r="412" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>121</v>
       </c>
@@ -18062,7 +18062,7 @@
         <v>15199150552</v>
       </c>
     </row>
-    <row r="413" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>33</v>
       </c>
@@ -18224,7 +18224,7 @@
         <v>17057071595</v>
       </c>
     </row>
-    <row r="419" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>189</v>
       </c>
@@ -18279,7 +18279,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="421" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>191</v>
       </c>
@@ -18302,7 +18302,7 @@
         <v>19056079999</v>
       </c>
     </row>
-    <row r="422" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>135</v>
       </c>
@@ -18328,7 +18328,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="423" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>35</v>
       </c>
@@ -18351,7 +18351,7 @@
         <v>19055754274</v>
       </c>
     </row>
-    <row r="424" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>35</v>
       </c>
@@ -18374,7 +18374,7 @@
         <v>19055754274</v>
       </c>
     </row>
-    <row r="425" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>35</v>
       </c>
@@ -18395,7 +18395,7 @@
       </c>
       <c r="I425"/>
     </row>
-    <row r="426" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>80</v>
       </c>
@@ -18418,7 +18418,7 @@
         <v>12267352666</v>
       </c>
     </row>
-    <row r="427" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>1339</v>
       </c>
@@ -18441,7 +18441,7 @@
         <v>12263962666</v>
       </c>
     </row>
-    <row r="428" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>60</v>
       </c>
@@ -18467,7 +18467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="429" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>214</v>
       </c>
@@ -18490,7 +18490,7 @@
         <v>17055165566</v>
       </c>
     </row>
-    <row r="430" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>95</v>
       </c>
@@ -18513,7 +18513,7 @@
         <v>19057279825</v>
       </c>
     </row>
-    <row r="431" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>60</v>
       </c>
@@ -18539,7 +18539,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="432" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>60</v>
       </c>
@@ -18562,7 +18562,7 @@
         <v>19054535454</v>
       </c>
     </row>
-    <row r="433" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>13</v>
       </c>
@@ -18585,7 +18585,7 @@
         <v>19056310001</v>
       </c>
     </row>
-    <row r="434" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
         <v>13</v>
       </c>
@@ -18608,7 +18608,7 @@
         <v>19053314441</v>
       </c>
     </row>
-    <row r="435" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>35</v>
       </c>
@@ -18631,7 +18631,7 @@
         <v>19055268130</v>
       </c>
     </row>
-    <row r="436" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>99</v>
       </c>
@@ -18654,7 +18654,7 @@
         <v>15196729826</v>
       </c>
     </row>
-    <row r="437" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>1355</v>
       </c>
@@ -18680,7 +18680,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="438" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
         <v>82</v>
       </c>
@@ -18703,7 +18703,7 @@
         <v>14167425050</v>
       </c>
     </row>
-    <row r="439" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>189</v>
       </c>
@@ -18726,7 +18726,7 @@
         <v>14379179399</v>
       </c>
     </row>
-    <row r="440" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>28</v>
       </c>
@@ -18752,7 +18752,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="441" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>28</v>
       </c>
@@ -18775,7 +18775,7 @@
         <v>14166076767</v>
       </c>
     </row>
-    <row r="442" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
         <v>28</v>
       </c>
@@ -18885,7 +18885,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="446" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
         <v>28</v>
       </c>
@@ -18908,7 +18908,7 @@
         <v>14165161116</v>
       </c>
     </row>
-    <row r="447" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>28</v>
       </c>
@@ -18931,7 +18931,7 @@
         <v>14165342304</v>
       </c>
     </row>
-    <row r="448" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
         <v>217</v>
       </c>
@@ -18957,7 +18957,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="449" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
         <v>50</v>
       </c>
@@ -19067,7 +19067,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="453" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
         <v>225</v>
       </c>
@@ -19090,7 +19090,7 @@
         <v>16134464461</v>
       </c>
     </row>
-    <row r="454" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
         <v>120</v>
       </c>
@@ -19139,7 +19139,7 @@
         <v>15199443180</v>
       </c>
     </row>
-    <row r="456" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
         <v>355</v>
       </c>
@@ -19165,7 +19165,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="457" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
         <v>135</v>
       </c>
@@ -19188,7 +19188,7 @@
         <v>12892967710</v>
       </c>
     </row>
-    <row r="458" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
         <v>105</v>
       </c>
@@ -19330,7 +19330,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="463" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
         <v>82</v>
       </c>
@@ -19353,7 +19353,7 @@
         <v>16472589957</v>
       </c>
     </row>
-    <row r="464" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
         <v>75</v>
       </c>
@@ -19376,7 +19376,7 @@
         <v>12892408338</v>
       </c>
     </row>
-    <row r="465" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
         <v>28</v>
       </c>
@@ -19402,7 +19402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="466" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
         <v>35</v>
       </c>
@@ -19428,7 +19428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="467" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>28</v>
       </c>
@@ -19480,7 +19480,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="469" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
         <v>28</v>
       </c>
@@ -19506,7 +19506,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="470" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
         <v>55</v>
       </c>
@@ -19555,7 +19555,7 @@
         <v>16133995777</v>
       </c>
     </row>
-    <row r="472" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
         <v>77</v>
       </c>
@@ -19581,7 +19581,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="473" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
         <v>885</v>
       </c>
@@ -19607,7 +19607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="474" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
         <v>489</v>
       </c>
@@ -19633,7 +19633,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="475" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
         <v>307</v>
       </c>
@@ -19659,7 +19659,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="476" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
         <v>28</v>
       </c>
@@ -19685,7 +19685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="477" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
         <v>60</v>
       </c>
@@ -19737,7 +19737,7 @@
         <v>19052161012</v>
       </c>
     </row>
-    <row r="479" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>60</v>
       </c>
@@ -19824,7 +19824,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="482" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
         <v>191</v>
       </c>
@@ -19850,7 +19850,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="483" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
         <v>1446</v>
       </c>
@@ -19876,7 +19876,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="484" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>1450</v>
       </c>
@@ -19902,7 +19902,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="485" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>134</v>
       </c>
@@ -19928,7 +19928,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="486" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
         <v>57</v>
       </c>
@@ -19954,7 +19954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="487" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
         <v>26</v>
       </c>
@@ -19980,7 +19980,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="488" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
         <v>28</v>
       </c>
@@ -20229,7 +20229,7 @@
         <v>16477953809</v>
       </c>
     </row>
-    <row r="497" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>1470</v>
       </c>
@@ -20368,7 +20368,7 @@
         <v>16133590100</v>
       </c>
     </row>
-    <row r="502" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
         <v>13</v>
       </c>
@@ -20391,7 +20391,7 @@
         <v>19053369191</v>
       </c>
     </row>
-    <row r="503" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>191</v>
       </c>
@@ -20417,7 +20417,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="504" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
         <v>28</v>
       </c>
@@ -20443,7 +20443,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="505" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>96</v>
       </c>
@@ -20469,7 +20469,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="506" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>75</v>
       </c>
@@ -20492,7 +20492,7 @@
         <v>19055790650</v>
       </c>
     </row>
-    <row r="507" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>191</v>
       </c>
@@ -20515,7 +20515,7 @@
         <v>16473529551</v>
       </c>
     </row>
-    <row r="508" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>38</v>
       </c>
@@ -20541,7 +20541,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="509" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>82</v>
       </c>
@@ -20567,7 +20567,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="510" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>35</v>
       </c>
@@ -20593,7 +20593,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="511" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>60</v>
       </c>
@@ -20619,7 +20619,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="512" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
         <v>121</v>
       </c>
@@ -20642,7 +20642,7 @@
         <v>15192523933</v>
       </c>
     </row>
-    <row r="513" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>268</v>
       </c>
@@ -20665,7 +20665,7 @@
         <v>15758884343</v>
       </c>
     </row>
-    <row r="514" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>28</v>
       </c>
@@ -20691,7 +20691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="515" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>1540</v>
       </c>
@@ -20717,7 +20717,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="516" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>810</v>
       </c>
@@ -20850,7 +20850,7 @@
         <v>12262530859</v>
       </c>
     </row>
-    <row r="521" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
         <v>135</v>
       </c>
@@ -21006,7 +21006,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="527" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A527" t="s">
         <v>177</v>
       </c>
@@ -21029,7 +21029,7 @@
         <v>15194773336</v>
       </c>
     </row>
-    <row r="528" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A528" t="s">
         <v>564</v>
       </c>
@@ -21055,7 +21055,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="529" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
         <v>60</v>
       </c>
@@ -21107,7 +21107,7 @@
         <v>16133722272</v>
       </c>
     </row>
-    <row r="531" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
         <v>76</v>
       </c>
@@ -21133,7 +21133,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="532" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
         <v>51</v>
       </c>
@@ -21159,7 +21159,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="533" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
         <v>191</v>
       </c>
@@ -21237,7 +21237,7 @@
         <v>19054956454</v>
       </c>
     </row>
-    <row r="536" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
         <v>82</v>
       </c>
@@ -21263,7 +21263,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="537" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
         <v>99</v>
       </c>
@@ -21396,7 +21396,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="542" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="542" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A542" t="s">
         <v>28</v>
       </c>
@@ -21422,7 +21422,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="543" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
         <v>487</v>
       </c>
@@ -21474,7 +21474,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="545" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
         <v>1089</v>
       </c>
@@ -21526,7 +21526,7 @@
         <v>12892982856</v>
       </c>
     </row>
-    <row r="547" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
         <v>1597</v>
       </c>
@@ -21549,7 +21549,7 @@
         <v>18072930010</v>
       </c>
     </row>
-    <row r="548" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A548" t="s">
         <v>41</v>
       </c>
@@ -21601,7 +21601,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="550" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A550" t="s">
         <v>135</v>
       </c>
@@ -21761,7 +21761,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="556" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A556" t="s">
         <v>135</v>
       </c>
@@ -21787,7 +21787,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="557" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A557" t="s">
         <v>95</v>
       </c>
@@ -21813,7 +21813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="558" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A558" t="s">
         <v>35</v>
       </c>
@@ -21839,7 +21839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="559" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="559" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A559" t="s">
         <v>51</v>
       </c>
@@ -21865,7 +21865,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="560" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="560" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A560" t="s">
         <v>55</v>
       </c>
@@ -21891,7 +21891,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="561" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A561" t="s">
         <v>35</v>
       </c>
@@ -21917,7 +21917,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="562" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="562" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A562" t="s">
         <v>1657</v>
       </c>
@@ -21943,7 +21943,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="563" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="563" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A563" t="s">
         <v>35</v>
       </c>
@@ -21966,7 +21966,7 @@
         <v>19053089444</v>
       </c>
     </row>
-    <row r="564" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="564" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A564" t="s">
         <v>35</v>
       </c>
@@ -22160,7 +22160,7 @@
         <v>16478079072</v>
       </c>
     </row>
-    <row r="571" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="571" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
         <v>95</v>
       </c>
@@ -22186,7 +22186,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="572" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="572" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A572" t="s">
         <v>64</v>
       </c>
@@ -22212,7 +22212,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="573" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="573" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
         <v>51</v>
       </c>
@@ -22238,7 +22238,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="574" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="574" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A574" t="s">
         <v>184</v>
       </c>
@@ -22264,7 +22264,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="575" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="575" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
         <v>326</v>
       </c>
@@ -22287,7 +22287,7 @@
         <v>17052426550</v>
       </c>
     </row>
-    <row r="576" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="576" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A576" t="s">
         <v>82</v>
       </c>
@@ -22313,7 +22313,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="577" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="577" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
         <v>38</v>
       </c>
@@ -22336,7 +22336,7 @@
         <v>14162826555</v>
       </c>
     </row>
-    <row r="578" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
         <v>51</v>
       </c>
@@ -22362,7 +22362,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="579" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
         <v>386</v>
       </c>
@@ -22388,7 +22388,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="580" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
         <v>26</v>
       </c>
@@ -22411,7 +22411,7 @@
         <v>12894820461</v>
       </c>
     </row>
-    <row r="581" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
         <v>50</v>
       </c>
@@ -22434,7 +22434,7 @@
         <v>16132300623</v>
       </c>
     </row>
-    <row r="582" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
         <v>50</v>
       </c>
@@ -22457,7 +22457,7 @@
         <v>16133199992</v>
       </c>
     </row>
-    <row r="583" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
         <v>659</v>
       </c>
@@ -22480,7 +22480,7 @@
         <v>12892251000</v>
       </c>
     </row>
-    <row r="584" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
         <v>38</v>
       </c>
@@ -22506,7 +22506,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="585" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
         <v>73</v>
       </c>
@@ -22529,7 +22529,7 @@
         <v>18076989753</v>
       </c>
     </row>
-    <row r="586" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
         <v>73</v>
       </c>
@@ -22552,7 +22552,7 @@
         <v>18076989753</v>
       </c>
     </row>
-    <row r="587" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
         <v>28</v>
       </c>
@@ -22572,7 +22572,7 @@
         <v>16473669030</v>
       </c>
     </row>
-    <row r="588" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
         <v>135</v>
       </c>
@@ -22595,7 +22595,7 @@
         <v>12899329413</v>
       </c>
     </row>
-    <row r="589" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
         <v>355</v>
       </c>
@@ -22615,7 +22615,7 @@
         <v>17164658787</v>
       </c>
     </row>
-    <row r="590" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
         <v>75</v>
       </c>
@@ -22638,7 +22638,7 @@
         <v>19052409378</v>
       </c>
     </row>
-    <row r="591" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
         <v>899</v>
       </c>
@@ -22664,7 +22664,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="592" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A592" t="s">
         <v>26</v>
       </c>
@@ -22690,7 +22690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="593" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="593" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A593" t="s">
         <v>26</v>
       </c>
@@ -22716,7 +22716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="594" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="594" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A594" t="s">
         <v>215</v>
       </c>
@@ -22739,7 +22739,7 @@
         <v>19057780668</v>
       </c>
     </row>
-    <row r="595" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="595" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A595" t="s">
         <v>548</v>
       </c>
@@ -22762,7 +22762,7 @@
         <v>16133420420</v>
       </c>
     </row>
-    <row r="596" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="596" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A596" t="s">
         <v>13</v>
       </c>
@@ -22785,7 +22785,7 @@
         <v>12892451787</v>
       </c>
     </row>
-    <row r="597" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="597" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
         <v>1487</v>
       </c>
@@ -22808,7 +22808,7 @@
         <v>15196693979</v>
       </c>
     </row>
-    <row r="598" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
         <v>78</v>
       </c>
@@ -22834,7 +22834,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="599" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="599" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
         <v>1742</v>
       </c>
@@ -22857,7 +22857,7 @@
         <v>12896749666</v>
       </c>
     </row>
-    <row r="600" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="600" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
         <v>250</v>
       </c>
@@ -22880,7 +22880,7 @@
         <v>14165918800</v>
       </c>
     </row>
-    <row r="601" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="601" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
         <v>28</v>
       </c>
@@ -22903,7 +22903,7 @@
         <v>14165918800</v>
       </c>
     </row>
-    <row r="602" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="602" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A602" t="s">
         <v>243</v>
       </c>
@@ -22926,7 +22926,7 @@
         <v>19054764464</v>
       </c>
     </row>
-    <row r="603" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="603" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
         <v>65</v>
       </c>
@@ -22949,7 +22949,7 @@
         <v>16133897420</v>
       </c>
     </row>
-    <row r="604" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="604" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A604" t="s">
         <v>99</v>
       </c>
@@ -22975,7 +22975,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="605" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="605" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
         <v>99</v>
       </c>
@@ -22998,7 +22998,7 @@
         <v>15196490444</v>
       </c>
     </row>
-    <row r="606" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="606" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A606" t="s">
         <v>64</v>
       </c>
@@ -23021,7 +23021,7 @@
         <v>17054785778</v>
       </c>
     </row>
-    <row r="607" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="607" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A607" t="s">
         <v>1761</v>
       </c>
@@ -23044,7 +23044,7 @@
         <v>14167390420</v>
       </c>
     </row>
-    <row r="608" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="608" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A608" t="s">
         <v>50</v>
       </c>
@@ -23067,7 +23067,7 @@
         <v>16134404200</v>
       </c>
     </row>
-    <row r="609" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="609" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A609" t="s">
         <v>51</v>
       </c>
@@ -23090,7 +23090,7 @@
         <v>16135655959</v>
       </c>
     </row>
-    <row r="610" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="610" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A610" t="s">
         <v>91</v>
       </c>
@@ -23113,7 +23113,7 @@
         <v>16138349200</v>
       </c>
     </row>
-    <row r="611" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="611" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A611" t="s">
         <v>88</v>
       </c>
@@ -23136,7 +23136,7 @@
         <v>17057431884</v>
       </c>
     </row>
-    <row r="612" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="612" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A612" t="s">
         <v>189</v>
       </c>
@@ -23162,7 +23162,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="613" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="613" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A613" t="s">
         <v>511</v>
       </c>
@@ -23188,7 +23188,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="614" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="614" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A614" t="s">
         <v>1527</v>
       </c>
@@ -23211,7 +23211,7 @@
         <v>15199258787</v>
       </c>
     </row>
-    <row r="615" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="615" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A615" t="s">
         <v>394</v>
       </c>
@@ -23234,7 +23234,7 @@
         <v>19056425111</v>
       </c>
     </row>
-    <row r="616" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="616" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A616" t="s">
         <v>1788</v>
       </c>
@@ -23260,7 +23260,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="617" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="617" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A617" t="s">
         <v>341</v>
       </c>
@@ -23283,7 +23283,7 @@
         <v>15192073400</v>
       </c>
     </row>
-    <row r="618" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="618" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A618" t="s">
         <v>73</v>
       </c>
@@ -23309,7 +23309,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="619" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="619" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A619" t="s">
         <v>82</v>
       </c>
@@ -23332,7 +23332,7 @@
         <v>16473688519</v>
       </c>
     </row>
-    <row r="620" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="620" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A620" t="s">
         <v>121</v>
       </c>
@@ -23355,7 +23355,7 @@
         <v>15199740600</v>
       </c>
     </row>
-    <row r="621" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="621" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A621" t="s">
         <v>53</v>
       </c>
@@ -23459,7 +23459,7 @@
         <v>15199255523</v>
       </c>
     </row>
-    <row r="625" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="625" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A625" t="s">
         <v>135</v>
       </c>
@@ -23482,7 +23482,7 @@
         <v>12892960915</v>
       </c>
     </row>
-    <row r="626" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="626" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A626" t="s">
         <v>548</v>
       </c>
@@ -23505,7 +23505,7 @@
         <v>16134997688</v>
       </c>
     </row>
-    <row r="627" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="627" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A627" t="s">
         <v>76</v>
       </c>
@@ -23531,7 +23531,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="628" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="628" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A628" t="s">
         <v>63</v>
       </c>
@@ -23557,7 +23557,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="629" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="629" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A629" t="s">
         <v>51</v>
       </c>
@@ -23632,7 +23632,7 @@
         <v>12893898989</v>
       </c>
     </row>
-    <row r="632" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="632" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A632" t="s">
         <v>28</v>
       </c>
@@ -23655,7 +23655,7 @@
         <v>14166932737</v>
       </c>
     </row>
-    <row r="633" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="633" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A633" t="s">
         <v>50</v>
       </c>
@@ -23681,7 +23681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="634" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="634" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A634" t="s">
         <v>191</v>
       </c>
@@ -23730,7 +23730,7 @@
         <v>14162669336</v>
       </c>
     </row>
-    <row r="636" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="636" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A636" t="s">
         <v>73</v>
       </c>
@@ -23756,7 +23756,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="637" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="637" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A637" t="s">
         <v>82</v>
       </c>
@@ -23834,7 +23834,7 @@
         <v>16139322525</v>
       </c>
     </row>
-    <row r="640" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="640" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A640" t="s">
         <v>1079</v>
       </c>
@@ -23860,7 +23860,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="641" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="641" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A641" t="s">
         <v>809</v>
       </c>
@@ -23886,7 +23886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="642" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="642" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A642" t="s">
         <v>28</v>
       </c>
@@ -23912,7 +23912,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="643" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="643" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A643" t="s">
         <v>38</v>
       </c>
@@ -23938,7 +23938,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="644" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="644" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A644" t="s">
         <v>41</v>
       </c>
@@ -23961,7 +23961,7 @@
         <v>19058859172</v>
       </c>
     </row>
-    <row r="645" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="645" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A645" t="s">
         <v>118</v>
       </c>
@@ -23987,7 +23987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="646" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="646" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A646" t="s">
         <v>82</v>
       </c>
@@ -24013,7 +24013,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="647" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="647" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A647" t="s">
         <v>134</v>
       </c>
@@ -24039,7 +24039,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="648" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="648" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A648" t="s">
         <v>75</v>
       </c>
@@ -24065,7 +24065,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="649" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="649" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A649" t="s">
         <v>53</v>
       </c>
@@ -24091,7 +24091,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="650" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="650" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A650" t="s">
         <v>13</v>
       </c>
@@ -24114,7 +24114,7 @@
         <v>19053339992</v>
       </c>
     </row>
-    <row r="651" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="651" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A651" t="s">
         <v>368</v>
       </c>
@@ -24137,7 +24137,7 @@
         <v>15198047733</v>
       </c>
     </row>
-    <row r="652" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="652" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A652" t="s">
         <v>268</v>
       </c>
@@ -24189,7 +24189,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="654" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="654" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A654" t="s">
         <v>76</v>
       </c>
@@ -24212,7 +24212,7 @@
         <v>15198047733</v>
       </c>
     </row>
-    <row r="655" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="655" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A655" t="s">
         <v>26</v>
       </c>
@@ -24296,7 +24296,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="658" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="658" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A658" t="s">
         <v>484</v>
       </c>
@@ -24322,7 +24322,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="659" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="659" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A659" t="s">
         <v>60</v>
       </c>
@@ -24374,7 +24374,7 @@
         <v>16138282929</v>
       </c>
     </row>
-    <row r="661" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="661" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A661" t="s">
         <v>184</v>
       </c>
@@ -24400,7 +24400,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="662" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="662" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A662" t="s">
         <v>1906</v>
       </c>
@@ -24565,7 +24565,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="668" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="668" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A668" t="s">
         <v>1906</v>
       </c>
@@ -24591,7 +24591,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="669" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="669" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A669" t="s">
         <v>121</v>
       </c>
@@ -24617,7 +24617,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="670" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="670" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A670" t="s">
         <v>60</v>
       </c>
@@ -24698,7 +24698,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="673" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="673" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A673" t="s">
         <v>95</v>
       </c>
@@ -24724,7 +24724,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="674" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="674" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A674" t="s">
         <v>35</v>
       </c>
@@ -24750,7 +24750,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="675" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="675" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A675" t="s">
         <v>1938</v>
       </c>
@@ -24776,7 +24776,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="676" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="676" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A676" t="s">
         <v>35</v>
       </c>
@@ -24802,7 +24802,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="677" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="677" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A677" t="s">
         <v>680</v>
       </c>
@@ -24825,7 +24825,7 @@
         <v>15195838420</v>
       </c>
     </row>
-    <row r="678" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="678" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A678" t="s">
         <v>1946</v>
       </c>
@@ -24880,7 +24880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="680" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="680" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A680" t="s">
         <v>1949</v>
       </c>
@@ -24903,7 +24903,7 @@
         <v>15192950105</v>
       </c>
     </row>
-    <row r="681" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="681" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A681" t="s">
         <v>191</v>
       </c>
@@ -24929,7 +24929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="682" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="682" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A682" t="s">
         <v>189</v>
       </c>
@@ -25080,7 +25080,7 @@
       </c>
       <c r="I687"/>
     </row>
-    <row r="688" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="688" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A688" t="s">
         <v>55</v>
       </c>
@@ -25100,7 +25100,7 @@
         <v>15197429366</v>
       </c>
     </row>
-    <row r="689" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="689" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A689" t="s">
         <v>296</v>
       </c>
@@ -25181,7 +25181,7 @@
       </c>
       <c r="I692"/>
     </row>
-    <row r="693" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="693" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A693" t="s">
         <v>1928</v>
       </c>
@@ -25199,7 +25199,7 @@
       </c>
       <c r="I693"/>
     </row>
-    <row r="694" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="694" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A694" t="s">
         <v>63</v>
       </c>
@@ -25217,7 +25217,7 @@
       </c>
       <c r="I694"/>
     </row>
-    <row r="695" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="695" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A695" t="s">
         <v>13</v>
       </c>
@@ -25256,7 +25256,7 @@
       </c>
       <c r="I696"/>
     </row>
-    <row r="697" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="697" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A697" t="s">
         <v>1991</v>
       </c>
@@ -25279,7 +25279,7 @@
         <v>15192089962</v>
       </c>
     </row>
-    <row r="698" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="698" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A698" t="s">
         <v>127</v>
       </c>
@@ -25299,7 +25299,7 @@
         <v>14167920466</v>
       </c>
     </row>
-    <row r="699" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="699" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A699" t="s">
         <v>1854</v>
       </c>
@@ -25317,7 +25317,7 @@
       </c>
       <c r="I699"/>
     </row>
-    <row r="700" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="700" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A700" t="s">
         <v>373</v>
       </c>
@@ -25335,7 +25335,7 @@
       </c>
       <c r="I700"/>
     </row>
-    <row r="701" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="701" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A701" t="s">
         <v>2005</v>
       </c>
@@ -25353,7 +25353,7 @@
       </c>
       <c r="I701"/>
     </row>
-    <row r="702" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="702" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A702" t="s">
         <v>442</v>
       </c>
@@ -25379,7 +25379,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="703" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="703" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A703" t="s">
         <v>403</v>
       </c>
@@ -25397,7 +25397,7 @@
       </c>
       <c r="I703"/>
     </row>
-    <row r="704" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="704" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A704" t="s">
         <v>564</v>
       </c>
@@ -25499,7 +25499,7 @@
       </c>
       <c r="I708"/>
     </row>
-    <row r="709" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="709" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A709" t="s">
         <v>28</v>
       </c>
@@ -25593,7 +25593,7 @@
       </c>
       <c r="I712"/>
     </row>
-    <row r="713" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="713" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A713" t="s">
         <v>28</v>
       </c>
@@ -25611,7 +25611,7 @@
       </c>
       <c r="I713"/>
     </row>
-    <row r="714" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="714" spans="1:10" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A714" t="s">
         <v>2043</v>
       </c>
@@ -25675,6 +25675,11 @@
   <autoFilter ref="A1:N716">
     <filterColumn colId="5">
       <filters blank="1"/>
+    </filterColumn>
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <hyperlinks>

</xml_diff>

<commit_message>
save Buddi test reporter
</commit_message>
<xml_diff>
--- a/platform_scrapper/data/cannabis_used_IDs.xlsx
+++ b/platform_scrapper/data/cannabis_used_IDs.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$300</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$300</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -3592,7 +3592,7 @@
   <dimension ref="A1:N300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -12048,6 +12048,7 @@
       <c r="I300"/>
     </row>
   </sheetData>
+  <autoFilter ref="F1:F300"/>
   <hyperlinks>
     <hyperlink ref="E17" r:id="rId1"/>
     <hyperlink ref="E69" r:id="rId2"/>

</xml_diff>

<commit_message>
restructure, save 1800 shops
</commit_message>
<xml_diff>
--- a/platform_scrapper/data/cannabis_used_IDs.xlsx
+++ b/platform_scrapper/data/cannabis_used_IDs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parsy\OneDrive\Desktop\DOT\cannabis-shops-scraping\platform_scrapper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{FD3100CF-290C-466A-9D45-3C977A621E58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{602E845E-660F-44C0-967A-4257ED24E0FF}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{FD3100CF-290C-466A-9D45-3C977A621E58}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{764D1F31-87D9-4BE0-9B5C-966C5FA8EF09}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2360,11 +2360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D178" sqref="D178"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2428,7 +2427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="2" spans="1:14" ht="14.4" customHeight="1">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -2457,7 +2456,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="3" spans="1:14" ht="14.4" customHeight="1">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -2486,7 +2485,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="4" spans="1:14" ht="14.4" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>51</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="5" spans="1:14" ht="14.4" customHeight="1">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -2547,7 +2546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="6" spans="1:14" ht="14.4" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>23</v>
       </c>
@@ -2583,7 +2582,7 @@
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="7" spans="1:14" ht="14.4" customHeight="1">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -2612,7 +2611,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="3" customFormat="1" ht="14.4" hidden="1" customHeight="1">
+    <row r="8" spans="1:14" s="3" customFormat="1" ht="14.4" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>208</v>
       </c>
@@ -2642,7 +2641,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="9" spans="1:14" ht="14.4" customHeight="1">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -2674,7 +2673,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="10" spans="1:14" ht="14.4" customHeight="1">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -2703,7 +2702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="11" spans="1:14" ht="14.4" customHeight="1">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2732,7 +2731,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="12" spans="1:14" ht="14.4" customHeight="1">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -2761,7 +2760,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="13" spans="1:14" ht="14.4" customHeight="1">
       <c r="A13" s="9" t="s">
         <v>108</v>
       </c>
@@ -2793,7 +2792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="14" spans="1:14" ht="14.4" customHeight="1">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -2822,7 +2821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="15" spans="1:14" ht="14.4" customHeight="1">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -2851,7 +2850,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="14.4" hidden="1" customHeight="1">
+    <row r="16" spans="1:14" ht="14.4" customHeight="1">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2880,7 +2879,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="9" customFormat="1" ht="14.4" hidden="1" customHeight="1">
+    <row r="17" spans="1:10" s="9" customFormat="1" ht="14.4" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>43</v>
       </c>
@@ -2912,7 +2911,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="18" spans="1:10" ht="14.4" customHeight="1">
       <c r="A18" t="s">
         <v>129</v>
       </c>
@@ -2941,7 +2940,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="19" spans="1:10" ht="14.4" customHeight="1">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -2970,7 +2969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="20" spans="1:10" ht="14.4" customHeight="1">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2999,7 +2998,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="21" spans="1:10" ht="14.4" customHeight="1">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -3028,7 +3027,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="22" spans="1:10" ht="14.4" customHeight="1">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -3057,7 +3056,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="23" spans="1:10" ht="14.4" customHeight="1">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -3086,7 +3085,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="24" spans="1:10" ht="14.4" customHeight="1">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -3115,7 +3114,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="25" spans="1:10" ht="14.4" customHeight="1">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -3144,7 +3143,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="26" spans="1:10" ht="14.4" customHeight="1">
       <c r="A26" t="s">
         <v>127</v>
       </c>
@@ -3173,7 +3172,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="27" spans="1:10" ht="14.4" customHeight="1">
       <c r="A27" t="s">
         <v>157</v>
       </c>
@@ -3202,7 +3201,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="28" spans="1:10" ht="14.4" customHeight="1">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -3231,7 +3230,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="29" spans="1:10" ht="14.4" customHeight="1">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -3260,7 +3259,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="30" spans="1:10" ht="14.4" customHeight="1">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -3289,7 +3288,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="31" spans="1:10" ht="14.4" customHeight="1">
       <c r="A31" t="s">
         <v>166</v>
       </c>
@@ -3318,7 +3317,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="32" spans="1:10" ht="14.4" customHeight="1">
       <c r="A32" t="s">
         <v>54</v>
       </c>
@@ -3347,7 +3346,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="33" spans="1:10" ht="14.4" customHeight="1">
       <c r="A33" t="s">
         <v>96</v>
       </c>
@@ -3405,7 +3404,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="35" spans="1:10" ht="14.4" customHeight="1">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -3434,7 +3433,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="36" spans="1:10" ht="14.4" customHeight="1">
       <c r="A36" t="s">
         <v>188</v>
       </c>
@@ -3463,7 +3462,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="37" spans="1:10" ht="14.4" customHeight="1">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -3492,7 +3491,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="38" spans="1:10" ht="14.4" customHeight="1">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -3521,7 +3520,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="39" spans="1:10" ht="14.4" customHeight="1">
       <c r="A39" t="s">
         <v>108</v>
       </c>
@@ -3550,7 +3549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="40" spans="1:10" ht="14.4" customHeight="1">
       <c r="A40" t="s">
         <v>133</v>
       </c>
@@ -3579,7 +3578,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="41" spans="1:10" ht="14.4" customHeight="1">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -3608,7 +3607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="42" spans="1:10" ht="14.4" customHeight="1">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -3637,7 +3636,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="43" spans="1:10" ht="14.4" customHeight="1">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -3666,7 +3665,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="44" spans="1:10" ht="14.4" customHeight="1">
       <c r="A44" t="s">
         <v>212</v>
       </c>
@@ -3695,7 +3694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="45" spans="1:10" ht="14.4" customHeight="1">
       <c r="A45" t="s">
         <v>101</v>
       </c>
@@ -3724,7 +3723,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="46" spans="1:10" ht="14.4" customHeight="1">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -3753,7 +3752,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="47" spans="1:10" ht="14.4" customHeight="1">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -3782,7 +3781,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="48" spans="1:10" ht="14.4" customHeight="1">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -3811,7 +3810,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="49" spans="1:10" ht="14.4" customHeight="1">
       <c r="A49" t="s">
         <v>231</v>
       </c>
@@ -3840,7 +3839,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="50" spans="1:10" ht="14.4" customHeight="1">
       <c r="A50" t="s">
         <v>27</v>
       </c>
@@ -3869,7 +3868,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="51" spans="1:10" ht="14.4" customHeight="1">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -3898,7 +3897,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="52" spans="1:10" ht="14.4" customHeight="1">
       <c r="A52" t="s">
         <v>240</v>
       </c>
@@ -3927,7 +3926,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="53" spans="1:10" ht="14.4" customHeight="1">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -3956,7 +3955,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="54" spans="1:10" ht="14.4" customHeight="1">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -3985,7 +3984,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="55" spans="1:10" ht="14.4" customHeight="1">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -4014,7 +4013,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="56" spans="1:10" ht="14.4" customHeight="1">
       <c r="A56" t="s">
         <v>223</v>
       </c>
@@ -4043,7 +4042,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="57" spans="1:10" ht="14.4" customHeight="1">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -4072,7 +4071,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="58" spans="1:10" ht="14.4" customHeight="1">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -4101,7 +4100,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="59" spans="1:10" ht="14.4" customHeight="1">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -4130,7 +4129,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="60" spans="1:10" ht="14.4" customHeight="1">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -4159,7 +4158,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="61" spans="1:10" ht="14.4" customHeight="1">
       <c r="A61" t="s">
         <v>27</v>
       </c>
@@ -4188,7 +4187,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="62" spans="1:10" ht="14.4" customHeight="1">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -4217,7 +4216,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="63" spans="1:10" ht="14.4" customHeight="1">
       <c r="A63" t="s">
         <v>264</v>
       </c>
@@ -4246,7 +4245,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="64" spans="1:10" ht="14.4" customHeight="1">
       <c r="A64" t="s">
         <v>51</v>
       </c>
@@ -4275,7 +4274,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="65" spans="1:11" ht="14.4" customHeight="1">
       <c r="A65" t="s">
         <v>51</v>
       </c>
@@ -4307,7 +4306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="66" spans="1:11" ht="14.4" customHeight="1">
       <c r="A66" t="s">
         <v>279</v>
       </c>
@@ -4336,7 +4335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="67" spans="1:11" ht="14.4" customHeight="1">
       <c r="A67" t="s">
         <v>283</v>
       </c>
@@ -4365,7 +4364,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="68" spans="1:11" ht="14.4" customHeight="1">
       <c r="A68" t="s">
         <v>287</v>
       </c>
@@ -4394,7 +4393,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="69" spans="1:11" ht="14.4" customHeight="1">
       <c r="A69" t="s">
         <v>25</v>
       </c>
@@ -4423,7 +4422,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="70" spans="1:11" ht="14.4" customHeight="1">
       <c r="A70" t="s">
         <v>63</v>
       </c>
@@ -4452,7 +4451,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="71" spans="1:11" ht="14.4" customHeight="1">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -4481,7 +4480,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="72" spans="1:11" ht="14.4" customHeight="1">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -4510,7 +4509,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="73" spans="1:11" ht="14.4" customHeight="1">
       <c r="A73" t="s">
         <v>23</v>
       </c>
@@ -4571,7 +4570,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="75" spans="1:11" ht="14.4" customHeight="1">
       <c r="A75" t="s">
         <v>51</v>
       </c>
@@ -4600,7 +4599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="76" spans="1:11" ht="14.4" customHeight="1">
       <c r="A76" t="s">
         <v>40</v>
       </c>
@@ -4629,7 +4628,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="77" spans="1:11" ht="14.4" customHeight="1">
       <c r="A77" t="s">
         <v>37</v>
       </c>
@@ -4658,7 +4657,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="78" spans="1:11" ht="14.4" customHeight="1">
       <c r="A78" t="s">
         <v>23</v>
       </c>
@@ -4687,7 +4686,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="79" spans="1:11" ht="14.4" customHeight="1">
       <c r="A79" t="s">
         <v>46</v>
       </c>
@@ -4713,7 +4712,7 @@
         <v>17057071595</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="80" spans="1:11" ht="14.4" customHeight="1">
       <c r="A80" t="s">
         <v>84</v>
       </c>
@@ -4742,7 +4741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="81" spans="1:11" ht="14.4" customHeight="1">
       <c r="A81" t="s">
         <v>65</v>
       </c>
@@ -4771,7 +4770,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="82" spans="1:11" ht="14.4" customHeight="1">
       <c r="A82" t="s">
         <v>177</v>
       </c>
@@ -4800,7 +4799,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="83" spans="1:11" ht="14.4" customHeight="1">
       <c r="A83" t="s">
         <v>36</v>
       </c>
@@ -4829,7 +4828,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="84" spans="1:11" ht="14.4" customHeight="1">
       <c r="A84" t="s">
         <v>23</v>
       </c>
@@ -4858,7 +4857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="85" spans="1:11" ht="14.4" customHeight="1">
       <c r="A85" t="s">
         <v>76</v>
       </c>
@@ -4887,7 +4886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="86" spans="1:11" ht="14.4" customHeight="1">
       <c r="A86" t="s">
         <v>23</v>
       </c>
@@ -4916,7 +4915,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="87" spans="1:11" ht="14.4" customHeight="1">
       <c r="A87" t="s">
         <v>43</v>
       </c>
@@ -4977,7 +4976,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="89" spans="1:11" ht="14.4" customHeight="1">
       <c r="A89" t="s">
         <v>43</v>
       </c>
@@ -5009,7 +5008,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="90" spans="1:11" ht="14.4" customHeight="1">
       <c r="A90" t="s">
         <v>43</v>
       </c>
@@ -5041,7 +5040,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="91" spans="1:11" ht="14.4" customHeight="1">
       <c r="A91" t="s">
         <v>23</v>
       </c>
@@ -5070,7 +5069,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="92" spans="1:11" ht="14.4" customHeight="1">
       <c r="A92" t="s">
         <v>86</v>
       </c>
@@ -5102,7 +5101,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="93" spans="1:11" ht="14.4" customHeight="1">
       <c r="A93" t="s">
         <v>85</v>
       </c>
@@ -5131,7 +5130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="94" spans="1:11" ht="14.4" customHeight="1">
       <c r="A94" t="s">
         <v>23</v>
       </c>
@@ -5160,7 +5159,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="95" spans="1:11" ht="14.4" customHeight="1">
       <c r="A95" t="s">
         <v>29</v>
       </c>
@@ -5189,7 +5188,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="96" spans="1:11" ht="14.4" customHeight="1">
       <c r="A96" t="s">
         <v>51</v>
       </c>
@@ -5218,7 +5217,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="97" spans="1:11" ht="14.4" customHeight="1">
       <c r="A97" t="s">
         <v>23</v>
       </c>
@@ -5247,7 +5246,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="98" spans="1:11" ht="14.4" customHeight="1">
       <c r="A98" t="s">
         <v>76</v>
       </c>
@@ -5308,7 +5307,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="100" spans="1:11" ht="14.4" customHeight="1">
       <c r="A100" t="s">
         <v>36</v>
       </c>
@@ -5337,7 +5336,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="101" spans="1:11" ht="14.4" customHeight="1">
       <c r="A101" t="s">
         <v>27</v>
       </c>
@@ -5363,7 +5362,7 @@
         <v>12892461172</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="102" spans="1:11" ht="14.4" customHeight="1">
       <c r="A102" t="s">
         <v>379</v>
       </c>
@@ -5389,7 +5388,7 @@
         <v>12262530859</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="103" spans="1:11" ht="14.4" customHeight="1">
       <c r="A103" t="s">
         <v>85</v>
       </c>
@@ -5415,7 +5414,7 @@
         <v>15193542255</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="104" spans="1:11" ht="14.4" customHeight="1">
       <c r="A104" t="s">
         <v>63</v>
       </c>
@@ -5441,7 +5440,7 @@
         <v>15192582544</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="105" spans="1:11" ht="14.4" customHeight="1">
       <c r="A105" t="s">
         <v>63</v>
       </c>
@@ -5467,7 +5466,7 @@
         <v>15192500712</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="106" spans="1:11" ht="14.4" customHeight="1">
       <c r="A106" t="s">
         <v>63</v>
       </c>
@@ -5522,7 +5521,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="108" spans="1:11" ht="14.4" customHeight="1">
       <c r="A108" t="s">
         <v>386</v>
       </c>
@@ -5577,7 +5576,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="110" spans="1:11" ht="14.4" customHeight="1">
       <c r="A110" t="s">
         <v>43</v>
       </c>
@@ -5603,7 +5602,7 @@
         <v>19054956454</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="111" spans="1:11" ht="14.4" customHeight="1">
       <c r="A111" t="s">
         <v>366</v>
       </c>
@@ -5629,7 +5628,7 @@
         <v>19054956454</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="14.4" hidden="1" customHeight="1">
+    <row r="112" spans="1:11" ht="14.4" customHeight="1">
       <c r="A112" t="s">
         <v>27</v>
       </c>
@@ -5655,7 +5654,7 @@
         <v>19055288955</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="113" spans="1:10" ht="14.4" customHeight="1">
       <c r="A113" t="s">
         <v>45</v>
       </c>
@@ -5681,7 +5680,7 @@
         <v>15197571001</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="114" spans="1:10" ht="14.4" customHeight="1">
       <c r="A114" t="s">
         <v>136</v>
       </c>
@@ -5710,7 +5709,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="115" spans="1:10" ht="14.4" customHeight="1">
       <c r="A115" t="s">
         <v>50</v>
       </c>
@@ -5739,7 +5738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="116" spans="1:10" ht="14.4" customHeight="1">
       <c r="A116" t="s">
         <v>405</v>
       </c>
@@ -5765,7 +5764,7 @@
         <v>12892982856</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="117" spans="1:10" ht="14.4" customHeight="1">
       <c r="A117" t="s">
         <v>180</v>
       </c>
@@ -5794,7 +5793,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="118" spans="1:10" ht="14.4" customHeight="1">
       <c r="A118" t="s">
         <v>38</v>
       </c>
@@ -5823,7 +5822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="119" spans="1:10" ht="14.4" customHeight="1">
       <c r="A119" t="s">
         <v>45</v>
       </c>
@@ -5849,7 +5848,7 @@
         <v>15193040660</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="120" spans="1:10" ht="14.4" customHeight="1">
       <c r="A120" t="s">
         <v>207</v>
       </c>
@@ -5875,7 +5874,7 @@
         <v>17058879567</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="121" spans="1:10" ht="14.4" customHeight="1">
       <c r="A121" t="s">
         <v>23</v>
       </c>
@@ -5899,7 +5898,7 @@
       </c>
       <c r="I121"/>
     </row>
-    <row r="122" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="122" spans="1:10" ht="14.4" customHeight="1">
       <c r="A122" t="s">
         <v>58</v>
       </c>
@@ -5928,7 +5927,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="123" spans="1:10" ht="14.4" customHeight="1">
       <c r="A123" t="s">
         <v>66</v>
       </c>
@@ -5957,7 +5956,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="124" spans="1:10" ht="14.4" customHeight="1">
       <c r="A124" t="s">
         <v>23</v>
       </c>
@@ -5986,7 +5985,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="125" spans="1:10" ht="14.4" customHeight="1">
       <c r="A125" t="s">
         <v>23</v>
       </c>
@@ -6015,7 +6014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="126" spans="1:10" ht="14.4" customHeight="1">
       <c r="A126" t="s">
         <v>51</v>
       </c>
@@ -6044,7 +6043,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="127" spans="1:10" ht="14.4" customHeight="1">
       <c r="A127" t="s">
         <v>81</v>
       </c>
@@ -6073,7 +6072,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="128" spans="1:10" ht="14.4" customHeight="1">
       <c r="A128" t="s">
         <v>23</v>
       </c>
@@ -6099,7 +6098,7 @@
         <v>16478079072</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="129" spans="1:10" ht="14.4" customHeight="1">
       <c r="A129" t="s">
         <v>21</v>
       </c>
@@ -6128,7 +6127,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="130" spans="1:10" ht="14.4" customHeight="1">
       <c r="A130" t="s">
         <v>71</v>
       </c>
@@ -6157,7 +6156,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="131" spans="1:10" ht="14.4" customHeight="1">
       <c r="A131" t="s">
         <v>80</v>
       </c>
@@ -6183,7 +6182,7 @@
         <v>15198210555</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="132" spans="1:10" ht="14.4" customHeight="1">
       <c r="A132" t="s">
         <v>366</v>
       </c>
@@ -6209,7 +6208,7 @@
         <v>15199255523</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="133" spans="1:10" ht="14.4" customHeight="1">
       <c r="A133" t="s">
         <v>45</v>
       </c>
@@ -6238,7 +6237,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="134" spans="1:10" ht="14.4" customHeight="1">
       <c r="A134" t="s">
         <v>27</v>
       </c>
@@ -6264,7 +6263,7 @@
         <v>12893896889</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="135" spans="1:10" ht="14.4" customHeight="1">
       <c r="A135" t="s">
         <v>27</v>
       </c>
@@ -6290,7 +6289,7 @@
         <v>12893898989</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="136" spans="1:10" ht="14.4" customHeight="1">
       <c r="A136" t="s">
         <v>29</v>
       </c>
@@ -6345,7 +6344,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="138" spans="1:10" ht="14.4" customHeight="1">
       <c r="A138" t="s">
         <v>65</v>
       </c>
@@ -6374,7 +6373,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="139" spans="1:10" ht="14.4" customHeight="1">
       <c r="A139" t="s">
         <v>65</v>
       </c>
@@ -6400,7 +6399,7 @@
         <v>16139322525</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="140" spans="1:10" ht="14.4" customHeight="1">
       <c r="A140" t="s">
         <v>278</v>
       </c>
@@ -6429,7 +6428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="141" spans="1:10" ht="14.4" customHeight="1">
       <c r="A141" t="s">
         <v>62</v>
       </c>
@@ -6458,7 +6457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="142" spans="1:10" ht="14.4" customHeight="1">
       <c r="A142" t="s">
         <v>71</v>
       </c>
@@ -6487,7 +6486,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="143" spans="1:10" ht="14.4" customHeight="1">
       <c r="A143" t="s">
         <v>49</v>
       </c>
@@ -6516,7 +6515,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="144" spans="1:10" ht="14.4" customHeight="1">
       <c r="A144" t="s">
         <v>38</v>
       </c>
@@ -6545,7 +6544,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="145" spans="1:10" ht="14.4" customHeight="1">
       <c r="A145" t="s">
         <v>63</v>
       </c>
@@ -6574,7 +6573,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="146" spans="1:10" ht="14.4" customHeight="1">
       <c r="A146" t="s">
         <v>483</v>
       </c>
@@ -6603,7 +6602,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="147" spans="1:10" ht="14.4" customHeight="1">
       <c r="A147" t="s">
         <v>35</v>
       </c>
@@ -6629,7 +6628,7 @@
         <v>16138282929</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="148" spans="1:10" ht="14.4" customHeight="1">
       <c r="A148" t="s">
         <v>122</v>
       </c>
@@ -6655,7 +6654,7 @@
         <v>13434760363</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="149" spans="1:10" ht="14.4" customHeight="1">
       <c r="A149" t="s">
         <v>25</v>
       </c>
@@ -6681,7 +6680,7 @@
         <v>14165219993</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="150" spans="1:10" ht="14.4" customHeight="1">
       <c r="A150" t="s">
         <v>43</v>
       </c>
@@ -6710,7 +6709,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="151" spans="1:10" ht="14.4" customHeight="1">
       <c r="A151" t="s">
         <v>29</v>
       </c>
@@ -6736,7 +6735,7 @@
         <v>14162910420</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="152" spans="1:10" ht="14.4" customHeight="1">
       <c r="A152" t="s">
         <v>36</v>
       </c>
@@ -6765,7 +6764,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="153" spans="1:10" ht="14.4" customHeight="1">
       <c r="A153" t="s">
         <v>55</v>
       </c>
@@ -6794,7 +6793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="154" spans="1:10" ht="14.4" customHeight="1">
       <c r="A154" t="s">
         <v>23</v>
       </c>
@@ -6852,7 +6851,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="156" spans="1:10" ht="14.4" customHeight="1">
       <c r="A156" t="s">
         <v>23</v>
       </c>
@@ -6881,7 +6880,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="157" spans="1:10" ht="14.4" customHeight="1">
       <c r="A157" t="s">
         <v>58</v>
       </c>
@@ -6907,7 +6906,7 @@
         <v>15196013420</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="158" spans="1:10" ht="14.4" customHeight="1">
       <c r="A158" t="s">
         <v>56</v>
       </c>
@@ -6933,7 +6932,7 @@
         <v>15196071966</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="159" spans="1:10" ht="14.4" customHeight="1">
       <c r="A159" t="s">
         <v>29</v>
       </c>
@@ -6962,7 +6961,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="160" spans="1:10" ht="14.4" customHeight="1">
       <c r="A160" t="s">
         <v>72</v>
       </c>
@@ -6983,7 +6982,7 @@
       </c>
       <c r="I160"/>
     </row>
-    <row r="161" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="161" spans="1:10" ht="14.4" customHeight="1">
       <c r="A161" t="s">
         <v>39</v>
       </c>
@@ -7006,7 +7005,7 @@
         <v>15197429366</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="162" spans="1:10" ht="14.4" customHeight="1">
       <c r="A162" t="s">
         <v>135</v>
       </c>
@@ -7027,7 +7026,7 @@
       </c>
       <c r="I162"/>
     </row>
-    <row r="163" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="163" spans="1:10" ht="14.4" customHeight="1">
       <c r="A163" t="s">
         <v>176</v>
       </c>
@@ -7048,7 +7047,7 @@
       </c>
       <c r="I163"/>
     </row>
-    <row r="164" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="164" spans="1:10" ht="14.4" customHeight="1">
       <c r="A164" t="s">
         <v>45</v>
       </c>
@@ -7069,7 +7068,7 @@
       </c>
       <c r="I164"/>
     </row>
-    <row r="165" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="165" spans="1:10" ht="14.4" customHeight="1">
       <c r="A165" t="s">
         <v>178</v>
       </c>
@@ -7090,7 +7089,7 @@
       </c>
       <c r="I165"/>
     </row>
-    <row r="166" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="166" spans="1:10" ht="14.4" customHeight="1">
       <c r="A166" t="s">
         <v>83</v>
       </c>
@@ -7111,7 +7110,7 @@
       </c>
       <c r="I166"/>
     </row>
-    <row r="167" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="167" spans="1:10" ht="14.4" customHeight="1">
       <c r="A167" t="s">
         <v>538</v>
       </c>
@@ -7132,7 +7131,7 @@
       </c>
       <c r="I167"/>
     </row>
-    <row r="168" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="168" spans="1:10" ht="14.4" customHeight="1">
       <c r="A168" t="s">
         <v>23</v>
       </c>
@@ -7153,7 +7152,7 @@
       </c>
       <c r="I168"/>
     </row>
-    <row r="169" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="169" spans="1:10" ht="14.4" customHeight="1">
       <c r="A169" t="s">
         <v>23</v>
       </c>
@@ -7174,7 +7173,7 @@
       </c>
       <c r="I169"/>
     </row>
-    <row r="170" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="170" spans="1:10" ht="14.4" customHeight="1">
       <c r="A170" t="s">
         <v>23</v>
       </c>
@@ -7195,7 +7194,7 @@
       </c>
       <c r="I170"/>
     </row>
-    <row r="171" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="171" spans="1:10" ht="14.4" customHeight="1">
       <c r="A171" t="s">
         <v>23</v>
       </c>
@@ -7221,7 +7220,7 @@
         <v>14165388225</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="172" spans="1:10" ht="14.4" customHeight="1">
       <c r="A172" t="s">
         <v>23</v>
       </c>
@@ -7242,7 +7241,7 @@
       </c>
       <c r="I172"/>
     </row>
-    <row r="173" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="173" spans="1:10" ht="14.4" customHeight="1">
       <c r="A173" t="s">
         <v>23</v>
       </c>
@@ -7271,7 +7270,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="174" spans="1:10" ht="14.4" customHeight="1">
       <c r="A174" t="s">
         <v>63</v>
       </c>
@@ -7292,7 +7291,7 @@
       </c>
       <c r="I174"/>
     </row>
-    <row r="175" spans="1:10" ht="14.4" hidden="1" customHeight="1">
+    <row r="175" spans="1:10" ht="14.4" customHeight="1">
       <c r="A175" t="s">
         <v>76</v>
       </c>
@@ -7314,30 +7313,7 @@
       <c r="I175"/>
     </row>
   </sheetData>
-  <autoFilter ref="F1:J175" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="['Delivery  within a 10km radius of our Waterloo store', 'Same-day delivery']"/>
-        <filter val="['Delivery  within a 20km radius of our Waterloo store', 'Same-day delivery']"/>
-        <filter val="['Delivery / Free Delivery within 12 kms']"/>
-        <filter val="['Delivery / free delivery within 7 KM', 'Same-day delivery']"/>
-        <filter val="['Delivery / need scan map', 'Same-day delivery']"/>
-        <filter val="['Delivery / scan map', 'Same-day delivery']"/>
-        <filter val="['Delivery / scan map']"/>
-        <filter val="['Delivery / We serve within 10 km radius.']"/>
-        <filter val="['Delivery 30km radium from 71 Broadway']"/>
-        <filter val="['Delivery in Courtice, Whitby, Oshawa', 'Same-day delivery']"/>
-        <filter val="['Delivery serve within 30 km radius', 'Same-day delivery']"/>
-        <filter val="['Delivery within 12 kms', 'Same-day delivery']"/>
-        <filter val="['Delivery within 25km', 'Same-day delivery']"/>
-        <filter val="['Delivery within 5 km radius.', 'Same-day delivery']"/>
-        <filter val="['Delivery within 50 km radius', 'Same-day delivery']"/>
-        <filter val="['Delivery within Arthur Ontario N0G 1A0']"/>
-        <filter val="['Delivery', 'Same-day delivery', 'We serve within 6 km radius']"/>
-        <filter val="['serve within 10 km radius, calculate', 'Delivery', 'Same-day delivery']"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="F1:J175" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="E28" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>

</xml_diff>